<commit_message>
README updated, report save and other functions updated - final commit
</commit_message>
<xml_diff>
--- a/reports/test_report.xlsx
+++ b/reports/test_report.xlsx
@@ -7,11 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="H1 Tag Existence" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="HTML Tag Sequence Test" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Image Alt Attribute Test" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="URL Status Test" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Currency Filter Test" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="HTML Tag Sequence Test" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Image Alt Attribute Test" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="URL Status Test" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Currency Filter Test" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Script Data Extraction Test" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="H1 Tag Existence" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,59 +430,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>testcase</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>result</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>comments</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>H1 Tag Existence</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>H1 tag exists</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -614,7 +562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1695,7 +1643,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Casa ecológica en Madrid</t>
+          <t>Desbloquee el mejor precio en Madrid</t>
         </is>
       </c>
     </row>
@@ -1729,7 +1677,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Ofertas por debajo de Hotala™ 149/semana</t>
+          <t>Gran oferta para esta noche</t>
         </is>
       </c>
     </row>
@@ -1763,7 +1711,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Bueno para parejas.  Libro Madrid</t>
+          <t>Descuento exclusivo para Madrid</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1745,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Casa de estilo único en Madrid</t>
+          <t>Tarifas calientes hoy.  Madrid Descuentos</t>
         </is>
       </c>
     </row>
@@ -1831,7 +1779,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Quédate en el corazón de Madrid</t>
+          <t>Bueno para las familias.  Libro Madrid</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1813,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Descuento exclusivo para Madrid</t>
+          <t>Villa de lujo a partir de Hotala™ 55</t>
         </is>
       </c>
     </row>
@@ -1993,7 +1941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2418,7 +2366,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-189483&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=0-BC-189483&amp;published=true&amp;dest_id=189483&amp;hero=BC-189483&amp;owner_id=189483&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2023-09-07T06%3A40%3A54.945897%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-189483&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=0-BC-189483&amp;published=true&amp;dest_id=189483&amp;hero=BC-189483&amp;owner_id=189483&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2023-09-07T06%3A40%3A54.945897%2B00%3A00</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2486,7 +2434,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-189483&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=0-BC-189483&amp;published=true&amp;dest_id=189483&amp;hero=BC-189483&amp;owner_id=189483&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2023-09-07T06%3A40%3A54.945897%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-189483&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=0-BC-189483&amp;published=true&amp;dest_id=189483&amp;hero=BC-189483&amp;owner_id=189483&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2023-09-07T06%3A40%3A54.945897%2B00%3A00</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2503,7 +2451,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-189483&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=0-BC-189483&amp;published=true&amp;dest_id=189483&amp;hero=BC-189483&amp;owner_id=189483&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2023-09-07T06%3A40%3A54.945897%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-189483&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=0-BC-189483&amp;published=true&amp;dest_id=189483&amp;hero=BC-189483&amp;owner_id=189483&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2023-09-07T06%3A40%3A54.945897%2B00%3A00</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2520,7 +2468,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156815498&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=1-HA-6156815498&amp;published=true&amp;dest_id=18772446&amp;hero=BC-189483&amp;owner_id=18772446&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-27T12%3A58%3A25.212854%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156815498&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=1-HA-6156815498&amp;published=true&amp;dest_id=18772446&amp;hero=BC-189483&amp;owner_id=18772446&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-27T12%3A58%3A25.212854%2B00%3A00</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2588,7 +2536,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156815498&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=1-HA-6156815498&amp;published=true&amp;dest_id=18772446&amp;hero=BC-189483&amp;owner_id=18772446&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-27T12%3A58%3A25.212854%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156815498&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=1-HA-6156815498&amp;published=true&amp;dest_id=18772446&amp;hero=BC-189483&amp;owner_id=18772446&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-27T12%3A58%3A25.212854%2B00%3A00</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2605,7 +2553,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156815498&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=1-HA-6156815498&amp;published=true&amp;dest_id=18772446&amp;hero=BC-189483&amp;owner_id=18772446&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-27T12%3A58%3A25.212854%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156815498&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=1-HA-6156815498&amp;published=true&amp;dest_id=18772446&amp;hero=BC-189483&amp;owner_id=18772446&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-27T12%3A58%3A25.212854%2B00%3A00</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2622,7 +2570,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10244095&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=2-BC-10244095&amp;published=true&amp;dest_id=10244095&amp;hero=BC-189483&amp;owner_id=10244095&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A20%3A22.500884%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10244095&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=2-BC-10244095&amp;published=true&amp;dest_id=10244095&amp;hero=BC-189483&amp;owner_id=10244095&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A20%3A22.500884%2B00%3A00</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2690,7 +2638,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10244095&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=2-BC-10244095&amp;published=true&amp;dest_id=10244095&amp;hero=BC-189483&amp;owner_id=10244095&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A20%3A22.500884%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10244095&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=2-BC-10244095&amp;published=true&amp;dest_id=10244095&amp;hero=BC-189483&amp;owner_id=10244095&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A20%3A22.500884%2B00%3A00</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2707,7 +2655,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10244095&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=2-BC-10244095&amp;published=true&amp;dest_id=10244095&amp;hero=BC-189483&amp;owner_id=10244095&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A20%3A22.500884%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10244095&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=2-BC-10244095&amp;published=true&amp;dest_id=10244095&amp;hero=BC-189483&amp;owner_id=10244095&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A20%3A22.500884%2B00%3A00</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2724,7 +2672,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6116948778&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=3-HA-6116948778&amp;published=true&amp;dest_id=18772116&amp;hero=BC-189483&amp;owner_id=18772116&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-12-04T09%3A56%3A47.681908%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6116948778&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=3-HA-6116948778&amp;published=true&amp;dest_id=18772116&amp;hero=BC-189483&amp;owner_id=18772116&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-12-04T09%3A56%3A47.681908%2B00%3A00</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2792,7 +2740,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6116948778&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=3-HA-6116948778&amp;published=true&amp;dest_id=18772116&amp;hero=BC-189483&amp;owner_id=18772116&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-12-04T09%3A56%3A47.681908%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6116948778&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=3-HA-6116948778&amp;published=true&amp;dest_id=18772116&amp;hero=BC-189483&amp;owner_id=18772116&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-12-04T09%3A56%3A47.681908%2B00%3A00</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2809,7 +2757,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6116948778&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=3-HA-6116948778&amp;published=true&amp;dest_id=18772116&amp;hero=BC-189483&amp;owner_id=18772116&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-12-04T09%3A56%3A47.681908%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6116948778&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=3-HA-6116948778&amp;published=true&amp;dest_id=18772116&amp;hero=BC-189483&amp;owner_id=18772116&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-12-04T09%3A56%3A47.681908%2B00%3A00</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2826,7 +2774,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12091357&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=4-BC-12091357&amp;published=true&amp;dest_id=12091357&amp;hero=BC-189483&amp;owner_id=12091357&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-30T04%3A41%3A52.792404%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12091357&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=4-BC-12091357&amp;published=true&amp;dest_id=12091357&amp;hero=BC-189483&amp;owner_id=12091357&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-30T04%3A41%3A52.792404%2B00%3A00</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2894,7 +2842,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12091357&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=4-BC-12091357&amp;published=true&amp;dest_id=12091357&amp;hero=BC-189483&amp;owner_id=12091357&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-30T04%3A41%3A52.792404%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12091357&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=4-BC-12091357&amp;published=true&amp;dest_id=12091357&amp;hero=BC-189483&amp;owner_id=12091357&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-30T04%3A41%3A52.792404%2B00%3A00</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2911,7 +2859,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12091357&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=4-BC-12091357&amp;published=true&amp;dest_id=12091357&amp;hero=BC-189483&amp;owner_id=12091357&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-30T04%3A41%3A52.792404%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12091357&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=4-BC-12091357&amp;published=true&amp;dest_id=12091357&amp;hero=BC-189483&amp;owner_id=12091357&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-30T04%3A41%3A52.792404%2B00%3A00</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2928,7 +2876,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156923934&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=5-HA-6156923934&amp;published=true&amp;dest_id=18977141&amp;hero=BC-189483&amp;owner_id=18977141&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-22T08%3A25%3A11.355906%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156923934&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=5-HA-6156923934&amp;published=true&amp;dest_id=18977141&amp;hero=BC-189483&amp;owner_id=18977141&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-22T08%3A25%3A11.355906%2B00%3A00</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2996,7 +2944,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156923934&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=5-HA-6156923934&amp;published=true&amp;dest_id=18977141&amp;hero=BC-189483&amp;owner_id=18977141&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-22T08%3A25%3A11.355906%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156923934&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=5-HA-6156923934&amp;published=true&amp;dest_id=18977141&amp;hero=BC-189483&amp;owner_id=18977141&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-22T08%3A25%3A11.355906%2B00%3A00</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -3013,7 +2961,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156923934&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=5-HA-6156923934&amp;published=true&amp;dest_id=18977141&amp;hero=BC-189483&amp;owner_id=18977141&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-22T08%3A25%3A11.355906%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156923934&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=5-HA-6156923934&amp;published=true&amp;dest_id=18977141&amp;hero=BC-189483&amp;owner_id=18977141&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;epc=c999&amp;upat=2024-11-22T08%3A25%3A11.355906%2B00%3A00</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -3030,7 +2978,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12840745&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=6-BC-12840745&amp;published=true&amp;dest_id=12840745&amp;hero=BC-189483&amp;owner_id=12840745&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-02T07%3A54%3A57.220817%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12840745&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=6-BC-12840745&amp;published=true&amp;dest_id=12840745&amp;hero=BC-189483&amp;owner_id=12840745&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-02T07%3A54%3A57.220817%2B00%3A00</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3098,7 +3046,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12840745&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=6-BC-12840745&amp;published=true&amp;dest_id=12840745&amp;hero=BC-189483&amp;owner_id=12840745&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-02T07%3A54%3A57.220817%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12840745&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=6-BC-12840745&amp;published=true&amp;dest_id=12840745&amp;hero=BC-189483&amp;owner_id=12840745&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-02T07%3A54%3A57.220817%2B00%3A00</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3115,7 +3063,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12840745&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=6-BC-12840745&amp;published=true&amp;dest_id=12840745&amp;hero=BC-189483&amp;owner_id=12840745&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-02T07%3A54%3A57.220817%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-12840745&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=6-BC-12840745&amp;published=true&amp;dest_id=12840745&amp;hero=BC-189483&amp;owner_id=12840745&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-02T07%3A54%3A57.220817%2B00%3A00</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3132,7 +3080,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156557057&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=7-HA-6156557057&amp;published=true&amp;dest_id=30666775&amp;hero=BC-189483&amp;owner_id=30666775&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-11-16T18%3A08%3A09.190473%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156557057&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=7-HA-6156557057&amp;published=true&amp;dest_id=30666775&amp;hero=BC-189483&amp;owner_id=30666775&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-11-16T18%3A08%3A09.190473%2B00%3A00</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3200,7 +3148,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156557057&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=7-HA-6156557057&amp;published=true&amp;dest_id=30666775&amp;hero=BC-189483&amp;owner_id=30666775&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-11-16T18%3A08%3A09.190473%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156557057&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=7-HA-6156557057&amp;published=true&amp;dest_id=30666775&amp;hero=BC-189483&amp;owner_id=30666775&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-11-16T18%3A08%3A09.190473%2B00%3A00</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3217,7 +3165,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156557057&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=7-HA-6156557057&amp;published=true&amp;dest_id=30666775&amp;hero=BC-189483&amp;owner_id=30666775&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-11-16T18%3A08%3A09.190473%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6156557057&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=7-HA-6156557057&amp;published=true&amp;dest_id=30666775&amp;hero=BC-189483&amp;owner_id=30666775&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-11-16T18%3A08%3A09.190473%2B00%3A00</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3234,7 +3182,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11696591&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=8-BC-11696591&amp;published=true&amp;dest_id=11696591&amp;hero=BC-189483&amp;owner_id=11696591&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T00%3A24%3A26.662445%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11696591&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=8-BC-11696591&amp;published=true&amp;dest_id=11696591&amp;hero=BC-189483&amp;owner_id=11696591&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T00%3A24%3A26.662445%2B00%3A00</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3302,7 +3250,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11696591&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=8-BC-11696591&amp;published=true&amp;dest_id=11696591&amp;hero=BC-189483&amp;owner_id=11696591&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T00%3A24%3A26.662445%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11696591&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=8-BC-11696591&amp;published=true&amp;dest_id=11696591&amp;hero=BC-189483&amp;owner_id=11696591&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T00%3A24%3A26.662445%2B00%3A00</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3319,7 +3267,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11696591&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=8-BC-11696591&amp;published=true&amp;dest_id=11696591&amp;hero=BC-189483&amp;owner_id=11696591&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T00%3A24%3A26.662445%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11696591&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=8-BC-11696591&amp;published=true&amp;dest_id=11696591&amp;hero=BC-189483&amp;owner_id=11696591&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T00%3A24%3A26.662445%2B00%3A00</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3336,7 +3284,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6158787924&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=9-HA-6158787924&amp;published=true&amp;dest_id=51322528&amp;hero=BC-189483&amp;owner_id=51322528&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-12-04T14%3A41%3A42.106824%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6158787924&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=9-HA-6158787924&amp;published=true&amp;dest_id=51322528&amp;hero=BC-189483&amp;owner_id=51322528&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-12-04T14%3A41%3A42.106824%2B00%3A00</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3404,7 +3352,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6158787924&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=9-HA-6158787924&amp;published=true&amp;dest_id=51322528&amp;hero=BC-189483&amp;owner_id=51322528&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-12-04T14%3A41%3A42.106824%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6158787924&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=9-HA-6158787924&amp;published=true&amp;dest_id=51322528&amp;hero=BC-189483&amp;owner_id=51322528&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-12-04T14%3A41%3A42.106824%2B00%3A00</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3421,7 +3369,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6158787924&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=9-HA-6158787924&amp;published=true&amp;dest_id=51322528&amp;hero=BC-189483&amp;owner_id=51322528&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-12-04T14%3A41%3A42.106824%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=12&amp;property_id=HA-6158787924&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=9-HA-6158787924&amp;published=true&amp;dest_id=51322528&amp;hero=BC-189483&amp;owner_id=51322528&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;epc=c999&amp;upat=2024-12-04T14%3A41%3A42.106824%2B00%3A00</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3438,7 +3386,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4798366&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=10-BC-4798366&amp;published=true&amp;dest_id=4798366&amp;hero=BC-189483&amp;owner_id=4798366&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-08-02T09%3A03%3A39.929774%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4798366&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=10-BC-4798366&amp;published=true&amp;dest_id=4798366&amp;hero=BC-189483&amp;owner_id=4798366&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-08-02T09%3A03%3A39.929774%2B00%3A00</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3506,7 +3454,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4798366&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=10-BC-4798366&amp;published=true&amp;dest_id=4798366&amp;hero=BC-189483&amp;owner_id=4798366&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-08-02T09%3A03%3A39.929774%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4798366&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=10-BC-4798366&amp;published=true&amp;dest_id=4798366&amp;hero=BC-189483&amp;owner_id=4798366&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-08-02T09%3A03%3A39.929774%2B00%3A00</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3523,7 +3471,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4798366&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=10-BC-4798366&amp;published=true&amp;dest_id=4798366&amp;hero=BC-189483&amp;owner_id=4798366&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-08-02T09%3A03%3A39.929774%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-4798366&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=10-BC-4798366&amp;published=true&amp;dest_id=4798366&amp;hero=BC-189483&amp;owner_id=4798366&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-08-02T09%3A03%3A39.929774%2B00%3A00</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3540,7 +3488,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11971039&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=11-BC-11971039&amp;published=true&amp;dest_id=11971039&amp;hero=BC-189483&amp;owner_id=11971039&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-29T17%3A01%3A30.066639%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11971039&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=11-BC-11971039&amp;published=true&amp;dest_id=11971039&amp;hero=BC-189483&amp;owner_id=11971039&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-29T17%3A01%3A30.066639%2B00%3A00</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3608,7 +3556,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11971039&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=11-BC-11971039&amp;published=true&amp;dest_id=11971039&amp;hero=BC-189483&amp;owner_id=11971039&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-29T17%3A01%3A30.066639%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11971039&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=11-BC-11971039&amp;published=true&amp;dest_id=11971039&amp;hero=BC-189483&amp;owner_id=11971039&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-29T17%3A01%3A30.066639%2B00%3A00</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -3625,7 +3573,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11971039&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=11-BC-11971039&amp;published=true&amp;dest_id=11971039&amp;hero=BC-189483&amp;owner_id=11971039&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-29T17%3A01%3A30.066639%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11971039&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=11-BC-11971039&amp;published=true&amp;dest_id=11971039&amp;hero=BC-189483&amp;owner_id=11971039&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-29T17%3A01%3A30.066639%2B00%3A00</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -3642,7 +3590,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-6732258&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=12-BC-6732258&amp;published=true&amp;dest_id=6732258&amp;hero=BC-189483&amp;owner_id=6732258&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-22T17%3A28%3A35.830550%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-6732258&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=12-BC-6732258&amp;published=true&amp;dest_id=6732258&amp;hero=BC-189483&amp;owner_id=6732258&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-22T17%3A28%3A35.830550%2B00%3A00</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -3710,7 +3658,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-6732258&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=12-BC-6732258&amp;published=true&amp;dest_id=6732258&amp;hero=BC-189483&amp;owner_id=6732258&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-22T17%3A28%3A35.830550%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-6732258&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=12-BC-6732258&amp;published=true&amp;dest_id=6732258&amp;hero=BC-189483&amp;owner_id=6732258&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-22T17%3A28%3A35.830550%2B00%3A00</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -3727,7 +3675,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-6732258&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=12-BC-6732258&amp;published=true&amp;dest_id=6732258&amp;hero=BC-189483&amp;owner_id=6732258&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-22T17%3A28%3A35.830550%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-6732258&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=12-BC-6732258&amp;published=true&amp;dest_id=6732258&amp;hero=BC-189483&amp;owner_id=6732258&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-11-22T17%3A28%3A35.830550%2B00%3A00</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -3744,7 +3692,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11793458&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=13-BC-11793458&amp;published=true&amp;dest_id=11793458&amp;hero=BC-189483&amp;owner_id=11793458&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T04%3A18%3A39.986668%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11793458&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=13-BC-11793458&amp;published=true&amp;dest_id=11793458&amp;hero=BC-189483&amp;owner_id=11793458&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T04%3A18%3A39.986668%2B00%3A00</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -3812,7 +3760,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11793458&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=13-BC-11793458&amp;published=true&amp;dest_id=11793458&amp;hero=BC-189483&amp;owner_id=11793458&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T04%3A18%3A39.986668%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11793458&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=13-BC-11793458&amp;published=true&amp;dest_id=11793458&amp;hero=BC-189483&amp;owner_id=11793458&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T04%3A18%3A39.986668%2B00%3A00</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -3829,7 +3777,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11793458&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=13-BC-11793458&amp;published=true&amp;dest_id=11793458&amp;hero=BC-189483&amp;owner_id=11793458&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T04%3A18%3A39.986668%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11793458&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=13-BC-11793458&amp;published=true&amp;dest_id=11793458&amp;hero=BC-189483&amp;owner_id=11793458&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-06T04%3A18%3A39.986668%2B00%3A00</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3846,7 +3794,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10045967&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=14-BC-10045967&amp;published=true&amp;dest_id=10045967&amp;hero=BC-189483&amp;owner_id=10045967&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-08T05%3A22%3A25.405442%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10045967&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=14-BC-10045967&amp;published=true&amp;dest_id=10045967&amp;hero=BC-189483&amp;owner_id=10045967&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-08T05%3A22%3A25.405442%2B00%3A00</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -3914,7 +3862,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10045967&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=14-BC-10045967&amp;published=true&amp;dest_id=10045967&amp;hero=BC-189483&amp;owner_id=10045967&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-08T05%3A22%3A25.405442%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10045967&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=14-BC-10045967&amp;published=true&amp;dest_id=10045967&amp;hero=BC-189483&amp;owner_id=10045967&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-08T05%3A22%3A25.405442%2B00%3A00</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3931,7 +3879,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10045967&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=14-BC-10045967&amp;published=true&amp;dest_id=10045967&amp;hero=BC-189483&amp;owner_id=10045967&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-08T05%3A22%3A25.405442%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10045967&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=14-BC-10045967&amp;published=true&amp;dest_id=10045967&amp;hero=BC-189483&amp;owner_id=10045967&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-08T05%3A22%3A25.405442%2B00%3A00</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3948,7 +3896,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10261738&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=15-BC-10261738&amp;published=true&amp;dest_id=10261738&amp;hero=BC-189483&amp;owner_id=10261738&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-20T17%3A57%3A46.499119%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10261738&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=15-BC-10261738&amp;published=true&amp;dest_id=10261738&amp;hero=BC-189483&amp;owner_id=10261738&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-20T17%3A57%3A46.499119%2B00%3A00</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -4016,7 +3964,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10261738&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=15-BC-10261738&amp;published=true&amp;dest_id=10261738&amp;hero=BC-189483&amp;owner_id=10261738&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-20T17%3A57%3A46.499119%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10261738&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=15-BC-10261738&amp;published=true&amp;dest_id=10261738&amp;hero=BC-189483&amp;owner_id=10261738&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-20T17%3A57%3A46.499119%2B00%3A00</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -4033,7 +3981,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10261738&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=15-BC-10261738&amp;published=true&amp;dest_id=10261738&amp;hero=BC-189483&amp;owner_id=10261738&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-20T17%3A57%3A46.499119%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10261738&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=15-BC-10261738&amp;published=true&amp;dest_id=10261738&amp;hero=BC-189483&amp;owner_id=10261738&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-20T17%3A57%3A46.499119%2B00%3A00</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -4050,7 +3998,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10238227&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=16-BC-10238227&amp;published=true&amp;dest_id=10238227&amp;hero=BC-189483&amp;owner_id=10238227&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-16T13%3A55%3A22.145391%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10238227&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=16-BC-10238227&amp;published=true&amp;dest_id=10238227&amp;hero=BC-189483&amp;owner_id=10238227&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-16T13%3A55%3A22.145391%2B00%3A00</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -4118,7 +4066,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10238227&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=16-BC-10238227&amp;published=true&amp;dest_id=10238227&amp;hero=BC-189483&amp;owner_id=10238227&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-16T13%3A55%3A22.145391%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10238227&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=16-BC-10238227&amp;published=true&amp;dest_id=10238227&amp;hero=BC-189483&amp;owner_id=10238227&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-16T13%3A55%3A22.145391%2B00%3A00</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -4135,7 +4083,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10238227&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=16-BC-10238227&amp;published=true&amp;dest_id=10238227&amp;hero=BC-189483&amp;owner_id=10238227&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-16T13%3A55%3A22.145391%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10238227&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=16-BC-10238227&amp;published=true&amp;dest_id=10238227&amp;hero=BC-189483&amp;owner_id=10238227&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-16T13%3A55%3A22.145391%2B00%3A00</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -4152,7 +4100,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-7405841&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=17-BC-7405841&amp;published=true&amp;dest_id=7405841&amp;hero=BC-189483&amp;owner_id=7405841&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T09%3A34%3A42.249727%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-7405841&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=17-BC-7405841&amp;published=true&amp;dest_id=7405841&amp;hero=BC-189483&amp;owner_id=7405841&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T09%3A34%3A42.249727%2B00%3A00</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -4220,7 +4168,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-7405841&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=17-BC-7405841&amp;published=true&amp;dest_id=7405841&amp;hero=BC-189483&amp;owner_id=7405841&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T09%3A34%3A42.249727%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-7405841&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=17-BC-7405841&amp;published=true&amp;dest_id=7405841&amp;hero=BC-189483&amp;owner_id=7405841&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T09%3A34%3A42.249727%2B00%3A00</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -4237,7 +4185,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-7405841&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=17-BC-7405841&amp;published=true&amp;dest_id=7405841&amp;hero=BC-189483&amp;owner_id=7405841&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T09%3A34%3A42.249727%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-7405841&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=17-BC-7405841&amp;published=true&amp;dest_id=7405841&amp;hero=BC-189483&amp;owner_id=7405841&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T09%3A34%3A42.249727%2B00%3A00</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -4254,7 +4202,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11389192&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=18-BC-11389192&amp;published=true&amp;dest_id=11389192&amp;hero=BC-189483&amp;owner_id=11389192&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-05T14%3A17%3A54.967391%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11389192&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=18-BC-11389192&amp;published=true&amp;dest_id=11389192&amp;hero=BC-189483&amp;owner_id=11389192&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-05T14%3A17%3A54.967391%2B00%3A00</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -4322,7 +4270,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11389192&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=18-BC-11389192&amp;published=true&amp;dest_id=11389192&amp;hero=BC-189483&amp;owner_id=11389192&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-05T14%3A17%3A54.967391%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11389192&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=18-BC-11389192&amp;published=true&amp;dest_id=11389192&amp;hero=BC-189483&amp;owner_id=11389192&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-05T14%3A17%3A54.967391%2B00%3A00</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4339,7 +4287,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11389192&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=18-BC-11389192&amp;published=true&amp;dest_id=11389192&amp;hero=BC-189483&amp;owner_id=11389192&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-05T14%3A17%3A54.967391%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11389192&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=18-BC-11389192&amp;published=true&amp;dest_id=11389192&amp;hero=BC-189483&amp;owner_id=11389192&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-07-05T14%3A17%3A54.967391%2B00%3A00</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -4356,7 +4304,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11723827&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=19-BC-11723827&amp;published=true&amp;dest_id=11723827&amp;hero=BC-189483&amp;owner_id=11723827&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-04T05%3A37%3A10.876905%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11723827&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=19-BC-11723827&amp;published=true&amp;dest_id=11723827&amp;hero=BC-189483&amp;owner_id=11723827&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-04T05%3A37%3A10.876905%2B00%3A00</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -4424,7 +4372,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11723827&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=19-BC-11723827&amp;published=true&amp;dest_id=11723827&amp;hero=BC-189483&amp;owner_id=11723827&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-04T05%3A37%3A10.876905%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11723827&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=19-BC-11723827&amp;published=true&amp;dest_id=11723827&amp;hero=BC-189483&amp;owner_id=11723827&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-04T05%3A37%3A10.876905%2B00%3A00</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4441,7 +4389,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11723827&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=19-BC-11723827&amp;published=true&amp;dest_id=11723827&amp;hero=BC-189483&amp;owner_id=11723827&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-04T05%3A37%3A10.876905%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-11723827&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=19-BC-11723827&amp;published=true&amp;dest_id=11723827&amp;hero=BC-189483&amp;owner_id=11723827&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-04T05%3A37%3A10.876905%2B00%3A00</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -4458,7 +4406,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5309144&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=20-BC-5309144&amp;published=true&amp;dest_id=5309144&amp;hero=BC-189483&amp;owner_id=5309144&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-12-01T19%3A04%3A06.713249%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5309144&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=20-BC-5309144&amp;published=true&amp;dest_id=5309144&amp;hero=BC-189483&amp;owner_id=5309144&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-12-01T19%3A04%3A06.713249%2B00%3A00</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -4526,7 +4474,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5309144&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=20-BC-5309144&amp;published=true&amp;dest_id=5309144&amp;hero=BC-189483&amp;owner_id=5309144&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-12-01T19%3A04%3A06.713249%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5309144&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=20-BC-5309144&amp;published=true&amp;dest_id=5309144&amp;hero=BC-189483&amp;owner_id=5309144&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-12-01T19%3A04%3A06.713249%2B00%3A00</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -4543,7 +4491,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5309144&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=20-BC-5309144&amp;published=true&amp;dest_id=5309144&amp;hero=BC-189483&amp;owner_id=5309144&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-12-01T19%3A04%3A06.713249%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-5309144&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=20-BC-5309144&amp;published=true&amp;dest_id=5309144&amp;hero=BC-189483&amp;owner_id=5309144&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-12-01T19%3A04%3A06.713249%2B00%3A00</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -4560,7 +4508,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-690497&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=21-BC-690497&amp;published=true&amp;dest_id=690497&amp;hero=BC-189483&amp;owner_id=690497&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-05T05%3A38%3A26.726420%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-690497&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=21-BC-690497&amp;published=true&amp;dest_id=690497&amp;hero=BC-189483&amp;owner_id=690497&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-05T05%3A38%3A26.726420%2B00%3A00</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -4628,7 +4576,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-690497&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=21-BC-690497&amp;published=true&amp;dest_id=690497&amp;hero=BC-189483&amp;owner_id=690497&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-05T05%3A38%3A26.726420%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-690497&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=21-BC-690497&amp;published=true&amp;dest_id=690497&amp;hero=BC-189483&amp;owner_id=690497&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-05T05%3A38%3A26.726420%2B00%3A00</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4645,7 +4593,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-690497&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=21-BC-690497&amp;published=true&amp;dest_id=690497&amp;hero=BC-189483&amp;owner_id=690497&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-05T05%3A38%3A26.726420%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-690497&amp;guests=2&amp;search_string=Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=21-BC-690497&amp;published=true&amp;dest_id=690497&amp;hero=BC-189483&amp;owner_id=690497&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-12-05T05%3A38%3A26.726420%2B00%3A00</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4662,7 +4610,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10597603&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=22-BC-10597603&amp;published=true&amp;dest_id=10597603&amp;hero=BC-189483&amp;owner_id=10597603&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-07-17T08%3A41%3A46.217812%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10597603&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=22-BC-10597603&amp;published=true&amp;dest_id=10597603&amp;hero=BC-189483&amp;owner_id=10597603&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-07-17T08%3A41%3A46.217812%2B00%3A00</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -4730,7 +4678,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10597603&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=22-BC-10597603&amp;published=true&amp;dest_id=10597603&amp;hero=BC-189483&amp;owner_id=10597603&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-07-17T08%3A41%3A46.217812%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10597603&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=22-BC-10597603&amp;published=true&amp;dest_id=10597603&amp;hero=BC-189483&amp;owner_id=10597603&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-07-17T08%3A41%3A46.217812%2B00%3A00</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4747,7 +4695,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10597603&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=22-BC-10597603&amp;published=true&amp;dest_id=10597603&amp;hero=BC-189483&amp;owner_id=10597603&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-07-17T08%3A41%3A46.217812%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10597603&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=22-BC-10597603&amp;published=true&amp;dest_id=10597603&amp;hero=BC-189483&amp;owner_id=10597603&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007&amp;upat=2024-07-17T08%3A41%3A46.217812%2B00%3A00</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4764,7 +4712,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10239029&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=23-BC-10239029&amp;published=true&amp;dest_id=10239029&amp;hero=BC-189483&amp;owner_id=10239029&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A14%3A36.430528%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10239029&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=23-BC-10239029&amp;published=true&amp;dest_id=10239029&amp;hero=BC-189483&amp;owner_id=10239029&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A14%3A36.430528%2B00%3A00</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -4832,7 +4780,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10239029&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=23-BC-10239029&amp;published=true&amp;dest_id=10239029&amp;hero=BC-189483&amp;owner_id=10239029&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A14%3A36.430528%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10239029&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=23-BC-10239029&amp;published=true&amp;dest_id=10239029&amp;hero=BC-189483&amp;owner_id=10239029&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A14%3A36.430528%2B00%3A00</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4849,7 +4797,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10239029&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=23-BC-10239029&amp;published=true&amp;dest_id=10239029&amp;hero=BC-189483&amp;owner_id=10239029&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A14%3A36.430528%2B00%3A00</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=BC-10239029&amp;guests=2&amp;search_string=Chueca,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=23-BC-10239029&amp;published=true&amp;dest_id=10239029&amp;hero=BC-189483&amp;owner_id=10239029&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=6053455&amp;upat=2024-11-26T10%3A14%3A36.430528%2B00%3A00</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4866,7 +4814,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=0-placeholder1&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=0-placeholder1&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4883,7 +4831,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=0-placeholder1&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=0-placeholder1&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4900,7 +4848,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=0-placeholder1&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder1&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=0-placeholder1&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4917,7 +4865,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=1-placeholder2&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=1-placeholder2&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4934,7 +4882,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=1-placeholder2&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=1-placeholder2&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4951,7 +4899,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=1-placeholder2&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder2&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=1-placeholder2&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4968,7 +4916,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=2-placeholder3&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=2-placeholder3&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4985,7 +4933,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=2-placeholder3&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=2-placeholder3&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -5002,7 +4950,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=2-placeholder3&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder3&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=2-placeholder3&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -5019,7 +4967,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=3-placeholder4&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=3-placeholder4&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -5036,7 +4984,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=3-placeholder4&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=3-placeholder4&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -5053,7 +5001,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=3-placeholder4&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder4&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=3-placeholder4&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -5070,7 +5018,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=4-placeholder5&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=4-placeholder5&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -5087,7 +5035,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=4-placeholder5&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=4-placeholder5&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -5104,7 +5052,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=4-placeholder5&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder5&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=4-placeholder5&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -5121,7 +5069,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=5-placeholder6&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=5-placeholder6&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -5138,7 +5086,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=5-placeholder6&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=5-placeholder6&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -5155,7 +5103,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733832290831&amp;referral_id=5-placeholder6&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
+          <t>https://www.alojamiento.io/redirect-partner?feed=11&amp;property_id=placeholder6&amp;guests=2&amp;search_string=Justicia,%20Madrid,%20Community%20of%20Madrid,%20Spain&amp;referrer_page=hybrid&amp;menu_id=1733890987713&amp;referral_id=5-placeholder6&amp;hero=BC-189483&amp;order=upsort_bh&amp;sqs=hybrid-default&amp;property_country=ES&amp;at=End-of-Result%20Ad&amp;eplId=553248635976399007</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -6509,6 +6457,178 @@
       <c r="C265" t="inlineStr">
         <is>
           <t>Status Code: 200</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>comment</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>$ US</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Currency $ US validated successfully.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>$ CA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Currency $ CA validated successfully.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>€ BE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Currency € BE validated successfully.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>£ IE</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Currency £ IE validated successfully.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>$ AU</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Currency $ AU validated successfully.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>$ SG</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Currency $ SG validated successfully.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>د.إ. AE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Currency د.إ. AE validated successfully.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>৳ BD</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Currency ৳ BD validated successfully.</t>
         </is>
       </c>
     </row>
@@ -6518,6 +6638,89 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>SiteURL</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>CampaignID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SiteName</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Browser</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://www.alojamiento.io</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ALOJAMIENTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>alo</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Firefox</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>BD</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>182.160.106.203</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6534,7 +6737,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>currency</t>
+          <t>testcase</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -6544,25 +6747,24 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>comment</t>
+          <t>comments</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>H1 Tag Existence</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: 
-</t>
+          <t>H1 tag exists</t>
         </is>
       </c>
     </row>

</xml_diff>